<commit_message>
feat (v0.2.0): Prepare steps before updating expectation_analyzes
</commit_message>
<xml_diff>
--- a/e_outputs/tidy long data export.xlsx
+++ b/e_outputs/tidy long data export.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>51225</v>
+        <v>51228</v>
       </c>
     </row>
     <row r="10">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>50483.16467409007</v>
+        <v>50486.91832131053</v>
       </c>
     </row>
     <row r="12">
@@ -836,7 +836,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>94932</v>
+        <v>94939</v>
       </c>
     </row>
     <row r="15">
@@ -1004,7 +1004,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>518392</v>
+        <v>518441</v>
       </c>
     </row>
     <row r="21">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>82891</v>
+        <v>82898</v>
       </c>
     </row>
     <row r="22">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>max of REGION_ORD_NUM</t>
+          <t>is_unique in COUNTRY_NAME</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1257,8 +1257,8 @@
           <t>Current</t>
         </is>
       </c>
-      <c r="F29" t="n">
-        <v>100</v>
+      <c r="F29" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Expectation</t>
+          <t>Current</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1305,16 +1305,16 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>min of REGION_ORD_NUM</t>
+          <t>max of REGION_ORD_NUM</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Current</t>
+          <t>Expectation</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Expectation</t>
+          <t>Current</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1361,18 +1361,16 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>unique in CURRENCY_CODE</t>
+          <t>min of REGION_ORD_NUM</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Current</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>GBP, EUR, ZAR, DKK, NOK, PLN, CZK, SEK, AED, USD</t>
-        </is>
+          <t>Expectation</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1386,22 +1384,22 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Table Analysis</t>
+          <t>Column Analysis</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>NOT_FROM_OPTIONS1</t>
+          <t>unique in CURRENCY_CODE</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Expectation</t>
+          <t>Current</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>FOR TABLE ANALYZES1</t>
+          <t>GBP, EUR, ZAR, DKK, NOK, PLN, CZK, SEK, AED, USD</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1419,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>NOT_FROM_OPTIONS2</t>
+          <t>NOT_FROM_OPTIONS1</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1431,7 +1429,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>FOR TABLE ANALYZES2</t>
+          <t>FOR TABLE ANALYZES1</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1449,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>NOT_FROM_OPTIONS3</t>
+          <t>NOT_FROM_OPTIONS2</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1461,7 +1459,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>FOR TABLE ANALYZES3</t>
+          <t>FOR TABLE ANALYZES2</t>
         </is>
       </c>
     </row>
@@ -1481,7 +1479,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>NOT_FROM_OPTIONS4</t>
+          <t>NOT_FROM_OPTIONS3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1491,7 +1489,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>FOR TABLE ANALYZES4</t>
+          <t>FOR TABLE ANALYZES3</t>
         </is>
       </c>
     </row>
@@ -1511,17 +1509,17 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>candidate_keys</t>
+          <t>NOT_FROM_OPTIONS4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Current</t>
+          <t>Expectation</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>COUNTRY_ID, COUNTRY_CODE, COUNTRY_NAME, COUNTRY_ORD_NUM</t>
+          <t>FOR TABLE ANALYZES4</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1544,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Expectation</t>
+          <t>Current</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1571,16 +1569,18 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>count_of_columns</t>
+          <t>candidate_keys</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Current</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>14</v>
+          <t>Expectation</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>COUNTRY_ID, COUNTRY_CODE, COUNTRY_NAME, COUNTRY_ORD_NUM</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1604,10 +1604,38 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>QA  VW DIM COUNTRY2</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Table Analysis</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>count_of_columns</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>Expectation</t>
         </is>
       </c>
-      <c r="F41" t="n">
+      <c r="F42" t="n">
         <v>14</v>
       </c>
     </row>

</xml_diff>